<commit_message>
Add row transformation and string case utilities
Introduced a new 'transform-row' operation for worksheet rows, supporting camelCase, PascalCase, snake_case, upper, and lower transformations. Refactored CMakeLists.txt to use a library target and enable Catch2-based tests, added unit tests for string case helpers, and updated example config and result files to demonstrate new features.
</commit_message>
<xml_diff>
--- a/example/input.xlsx
+++ b/example/input.xlsx
@@ -29,13 +29,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>No.</t>
+    <t>No</t>
   </si>
   <si>
-    <t>Code</t>
+    <t>Product-Code</t>
   </si>
   <si>
-    <t>Name</t>
+    <t>Product-Name</t>
   </si>
   <si>
     <t>VG-WHITE</t>
@@ -1208,8 +1208,8 @@
   <sheetPr/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
Add advanced operations: group, sort, renumber, remove column
Introduces new operations including group-collect-to-array, sort-rows-by-column, reassign-numbering, and remove-column. Updates the YAML config, documentation, and example outputs to demonstrate these features. Refactors main.cpp to provide detailed operation logs and timing. Adds fmt as a dependency for formatted output. Enhances json.hpp to better handle arrays and numbers in JSON output.
</commit_message>
<xml_diff>
--- a/example/input.xlsx
+++ b/example/input.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>No</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Product-Name</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
   <si>
     <t>VG-WHITE</t>
@@ -54,6 +57,12 @@
   </si>
   <si>
     <t>B Necklace</t>
+  </si>
+  <si>
+    <t>BN-RED</t>
+  </si>
+  <si>
+    <t>GH-BROWN</t>
   </si>
 </sst>
 </file>
@@ -1206,19 +1215,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="3"/>
   <cols>
     <col min="2" max="2" width="12.2421875" customWidth="1"/>
     <col min="3" max="3" width="11.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1228,38 +1237,78 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
+      <c r="D6">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add unique item option to group-collect operation
Introduces the 'mark-unique-items' option to the group-collect operation, allowing collected array values to be deduplicated. Updates documentation, config, and example outputs to reflect this new feature. Also improves operation summary output in main.cpp and bumps the package version to 0.1.11.
</commit_message>
<xml_diff>
--- a/example/input.xlsx
+++ b/example/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22240" windowHeight="12620"/>
+    <workbookView windowWidth="26840" windowHeight="13320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>No</t>
   </si>
@@ -1215,13 +1215,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
     <col min="2" max="2" width="12.2421875" customWidth="1"/>
     <col min="3" max="3" width="11.84375" customWidth="1"/>
@@ -1311,6 +1311,20 @@
         <v>300</v>
       </c>
     </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Refactor config to script, enhance split and fill logic
Renamed config.yaml to script.yaml and updated all references from 'config' to 'script' in code and documentation. Improved split-column operation to support three-way splits and per-row normalization, and enhanced fill-column to support conditional expressions with 'ifcol'. Updated example files and documentation to reflect new column structure and logic.
</commit_message>
<xml_diff>
--- a/example/input.xlsx
+++ b/example/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26840" windowHeight="13320"/>
+    <workbookView windowWidth="18100" windowHeight="13320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>Product-Code</t>
+    <t>Product-Size-Color</t>
   </si>
   <si>
     <t>Product-Name</t>
@@ -41,7 +41,7 @@
     <t>Price</t>
   </si>
   <si>
-    <t>VG-WHITE</t>
+    <t>VG-XS-WHITE</t>
   </si>
   <si>
     <t>V Shirt</t>
@@ -53,16 +53,19 @@
     <t>G Handbag</t>
   </si>
   <si>
-    <t>BN-PURPLE</t>
+    <t>BN-XS-PURPLE</t>
   </si>
   <si>
     <t>B Necklace</t>
   </si>
   <si>
-    <t>BN-RED</t>
+    <t>BN-S-RED</t>
   </si>
   <si>
     <t>GH-BROWN</t>
+  </si>
+  <si>
+    <t>GH-RED</t>
   </si>
 </sst>
 </file>
@@ -1218,7 +1221,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="3"/>
@@ -1316,7 +1319,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>

</xml_diff>